<commit_message>
min max salary in template
</commit_message>
<xml_diff>
--- a/lab1_template.xlsx
+++ b/lab1_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Расчет заработной платы сотрудников предприятия ООО "Изумруд"</t>
   </si>
@@ -52,55 +52,70 @@
     <t>Зам. директора</t>
   </si>
   <si>
-    <t>05.16.2003</t>
+    <t>02.08.2010</t>
   </si>
   <si>
     <t>Коробова П.Н</t>
   </si>
   <si>
+    <t>Менеджер</t>
+  </si>
+  <si>
+    <t>10.19.2005</t>
+  </si>
+  <si>
+    <t>Морозов И.Р.</t>
+  </si>
+  <si>
     <t>Водитель</t>
   </si>
   <si>
-    <t>10.02.2006</t>
-  </si>
-  <si>
-    <t>Морозов И.Р.</t>
+    <t>04.04.2008</t>
+  </si>
+  <si>
+    <t>Ромашова П.Т.</t>
+  </si>
+  <si>
+    <t>Секетарь</t>
+  </si>
+  <si>
+    <t>07.14.2008</t>
+  </si>
+  <si>
+    <t>Петров Г.Т.</t>
   </si>
   <si>
     <t>Бухгалтер</t>
   </si>
   <si>
-    <t>08.24.2002</t>
-  </si>
-  <si>
-    <t>Ромашова П.Т.</t>
-  </si>
-  <si>
-    <t>11.28.2011</t>
-  </si>
-  <si>
-    <t>Петров Г.Т.</t>
-  </si>
-  <si>
-    <t>Менеджер</t>
-  </si>
-  <si>
-    <t>10.14.2005</t>
+    <t>08.29.2011</t>
   </si>
   <si>
     <t>Смирнов С.И.</t>
   </si>
   <si>
-    <t>07.27.2005</t>
+    <t>Директор</t>
+  </si>
+  <si>
+    <t>06.05.2004</t>
   </si>
   <si>
     <t>Соколова О.С.</t>
   </si>
   <si>
-    <t>05.08.2007</t>
-  </si>
-  <si>
-    <t>Курс доллара</t>
+    <t>09.19.2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Курс доллара: </t>
+  </si>
+  <si>
+    <t>Средняя зарплата, руб:</t>
+  </si>
+  <si>
+    <t>Максимальная зарплата, руб:</t>
+  </si>
+  <si>
+    <t>Минимальная зарплата, руб:</t>
   </si>
 </sst>
 </file>
@@ -470,7 +485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:I14"/>
+  <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,7 +494,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="5"/>
-    <col customWidth="1" max="2" min="2" width="15"/>
+    <col customWidth="1" max="2" min="2" width="28"/>
     <col customWidth="1" max="3" min="3" width="16"/>
     <col customWidth="1" max="4" min="4" width="18"/>
     <col customWidth="1" max="5" min="5" width="18"/>
@@ -588,10 +603,10 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="n"/>
       <c r="F8" s="3" t="n"/>
@@ -604,13 +619,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="3" t="n"/>
       <c r="F9" s="3" t="n"/>
@@ -623,13 +638,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="n"/>
       <c r="F10" s="3" t="n"/>
@@ -642,13 +657,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="n"/>
       <c r="F11" s="3" t="n"/>
@@ -662,12 +677,30 @@
       <c r="I12" s="3" t="n"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>48</v>
-      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>41.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="n"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="n"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="2" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>